<commit_message>
organize and add to doc
</commit_message>
<xml_diff>
--- a/src/main/resources/Final Report/Report Assets/Tables_charts.xlsx
+++ b/src/main/resources/Final Report/Report Assets/Tables_charts.xlsx
@@ -5,18 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yenton/Documents/z.Desktop/CSC class/CSC340/Projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yenton/Documents/z.Desktop/CSC class/CSC340/Projects/CSB340_CPUScheduler/Tables:"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEE39E0-8529-044F-B9A1-ACA6B1E947D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF3613C-DFC4-0C4F-AD39-2B3409982D66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-84700" yWindow="-2760" windowWidth="32100" windowHeight="16940" xr2:uid="{19E4D0F0-A2E2-4642-87EC-355669AFD3C9}"/>
+    <workbookView xWindow="-89560" yWindow="-4800" windowWidth="36960" windowHeight="18980" activeTab="1" xr2:uid="{19E4D0F0-A2E2-4642-87EC-355669AFD3C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="2" r:id="rId1"/>
     <sheet name="Plots" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Plots!$A$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Plots!$B$1:$G$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Plots!$B$2:$G$2</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>FCFS - NonPre</t>
   </si>
@@ -118,9 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">MLQ CPU utilization: </t>
-  </si>
-  <si>
-    <t>63.13% </t>
   </si>
   <si>
     <t xml:space="preserve">MLFQ CPU utilization:  </t>
@@ -254,20 +259,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -284,6 +284,9 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +438,7 @@
                   <c:v>0.9294</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.63129999999999997</c:v>
+                  <c:v>0.95840599999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.93730000000000002</c:v>
@@ -518,6 +521,7 @@
         <c:axId val="1142907872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -780,7 +784,7 @@
                   <c:v>175.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>293.25</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>154</c:v>
@@ -1125,7 +1129,7 @@
                   <c:v>511.63</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>629.38</c:v>
+                  <c:v>484.125</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>490.13</c:v>
@@ -1470,7 +1474,7 @@
                   <c:v>15.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>264</c:v>
+                  <c:v>24.63</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>15.75</c:v>
@@ -3991,6 +3995,25 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Plots"/>
+      <sheetName val="Plots"/>
+      <sheetName val="Plots"/>
+      <sheetName val="Plots"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4290,8 +4313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBAD2DE-4DEF-254B-8987-A511958746C8}">
   <dimension ref="B4:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S8" sqref="M4:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4307,459 +4330,468 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:19" ht="34" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15" t="s">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="N4" s="14" t="s">
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="N4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12">
         <v>0.77980000000000005</v>
       </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="M5" s="4" t="s">
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="M5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="8">
         <v>0.85340000000000005</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="8">
         <v>0.82779999999999998</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="8">
         <v>0.77980000000000005</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="8">
         <v>0.9294</v>
       </c>
-      <c r="R5" s="13">
-        <v>0.63129999999999997</v>
-      </c>
-      <c r="S5" s="13">
+      <c r="R5" s="8">
+        <v>0.95840599999999998</v>
+      </c>
+      <c r="S5" s="8">
         <v>0.93730000000000002</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="4">
         <v>185.25</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="4">
         <v>133.5</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="4">
         <v>150.5</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="4">
         <v>175.5</v>
       </c>
-      <c r="R6" s="6">
-        <v>293.25</v>
-      </c>
-      <c r="S6" s="6">
+      <c r="R6" s="4">
+        <v>148</v>
+      </c>
+      <c r="S6" s="4">
         <v>154</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>170</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>395</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>0</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>43</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>268</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="6">
         <v>11</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="4">
         <v>73</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="5">
         <v>298</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="6">
         <v>27</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="5">
         <v>521.37</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="5">
         <v>469.62</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="5">
         <v>486.63</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="5">
         <v>511.63</v>
       </c>
-      <c r="R7" s="7">
-        <v>629.38</v>
-      </c>
-      <c r="S7" s="7">
+      <c r="R7" s="5">
+        <v>484.125</v>
+      </c>
+      <c r="S7" s="5">
         <v>490.13</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>164</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>591</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="6">
         <v>5</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>73</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>500</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="6">
         <v>3</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="4">
         <v>197</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="5">
         <v>624</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="6">
         <v>67</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="6">
         <v>24.37</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="6">
         <v>27.13</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8" s="6">
         <v>53.25</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="Q8" s="6">
         <v>15.75</v>
       </c>
-      <c r="R8" s="8">
-        <v>264</v>
-      </c>
-      <c r="S8" s="8">
+      <c r="R8" s="6">
+        <v>24.63</v>
+      </c>
+      <c r="S8" s="6">
         <v>15.75</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>165</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>557</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="6">
         <v>9</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <v>276</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="5">
         <v>668</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="6">
         <v>16</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="4">
         <v>157</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="5">
         <v>549</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="6">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>164</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>648</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="6">
         <v>17</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <v>50</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="5">
         <v>534</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="6">
         <v>0</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="4">
         <v>97</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="5">
         <v>581</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="6">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>221</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>530</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="6">
         <v>20</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="4">
         <v>237</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="5">
         <v>546</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="6">
         <v>109</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="4">
         <v>0</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="5">
         <v>309</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>230</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>445</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="6">
         <v>36</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <v>121</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="5">
         <v>336</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="6">
         <v>24</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="4">
         <v>50</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="5">
         <v>265</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="6">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <v>184</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>512</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="6">
         <v>47</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="4">
         <v>149</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="5">
         <v>477</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="6">
         <v>47</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="4">
         <v>381</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="5">
         <v>709</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="6">
         <v>158</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <v>184</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>493</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="6">
         <v>61</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="4">
         <v>119</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="5">
         <v>428</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="6">
         <v>7</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="4">
         <v>249</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="5">
         <v>558</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14" s="6">
         <v>91</v>
       </c>
-      <c r="O14" s="5"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="14">
+        <f>AVERAGE(C7:C14)</f>
         <v>185.25</v>
       </c>
-      <c r="D15" s="11">
-        <v>521.37</v>
-      </c>
-      <c r="E15" s="12">
-        <v>24.37</v>
-      </c>
-      <c r="F15" s="10">
+      <c r="D15" s="15">
+        <f>AVERAGE(D7:D14)</f>
+        <v>521.375</v>
+      </c>
+      <c r="E15" s="16">
+        <f>AVERAGE(E7:E14)</f>
+        <v>24.375</v>
+      </c>
+      <c r="F15" s="14">
+        <f>AVERAGE(F7:F14)</f>
         <v>133.5</v>
       </c>
-      <c r="G15" s="11">
-        <v>469.63</v>
-      </c>
-      <c r="H15" s="12">
-        <v>27.13</v>
-      </c>
-      <c r="I15" s="10">
+      <c r="G15" s="15">
+        <f>AVERAGE(G7:G14)</f>
+        <v>469.625</v>
+      </c>
+      <c r="H15" s="16">
+        <f>AVERAGE(H7:H14)</f>
+        <v>27.125</v>
+      </c>
+      <c r="I15" s="14">
+        <f>AVERAGE(I7:I14)</f>
         <v>150.5</v>
       </c>
-      <c r="J15" s="11">
-        <v>486.63</v>
-      </c>
-      <c r="K15" s="12">
+      <c r="J15" s="15">
+        <f>AVERAGE(J7:J14)</f>
+        <v>486.625</v>
+      </c>
+      <c r="K15" s="16">
+        <f>AVERAGE(K7:K14)</f>
         <v>53.25</v>
       </c>
     </row>
@@ -4767,372 +4799,381 @@
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15" t="s">
+      <c r="C18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
-      <c r="C19" s="18">
+      <c r="C19" s="13">
         <v>0.9294</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17">
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="11">
+        <v>95.84</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="12">
         <v>0.93730000000000002</v>
       </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="4">
         <v>107</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <v>332</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="6">
         <v>0</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="4">
         <v>15</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="5">
         <v>240</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="6">
         <v>0</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="4">
         <v>50</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="5">
         <v>275</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="4">
         <v>125</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="5">
         <v>552</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="6">
         <v>5</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <v>35</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="5">
         <v>462</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="6">
         <v>4</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="4">
         <v>134</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="5">
         <v>561</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K22" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="4">
         <v>203</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
         <v>595</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="6">
         <v>9</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="4">
         <v>57</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="5">
         <v>449</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="6">
         <v>8</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="4">
         <v>198</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="5">
         <v>590</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K23" s="6">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>88</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <v>572</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="6">
         <v>14</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="4">
         <v>17</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="5">
         <v>501</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="6">
         <v>12</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="4">
         <v>17</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="5">
         <v>501</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24" s="6">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="4">
         <v>255</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <v>564</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="6">
         <v>17</v>
       </c>
-      <c r="F25" s="6">
-        <v>542</v>
-      </c>
-      <c r="G25" s="7">
-        <v>851</v>
-      </c>
-      <c r="H25" s="8">
-        <v>501</v>
-      </c>
-      <c r="I25" s="6">
+      <c r="F25" s="4">
+        <v>268</v>
+      </c>
+      <c r="G25" s="5">
+        <v>577</v>
+      </c>
+      <c r="H25" s="6">
+        <v>20</v>
+      </c>
+      <c r="I25" s="4">
         <v>256</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="5">
         <v>565</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="4">
         <v>206</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="5">
         <v>421</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="6">
         <v>22</v>
       </c>
-      <c r="F26" s="6">
-        <v>576</v>
-      </c>
-      <c r="G26" s="7">
-        <v>791</v>
-      </c>
-      <c r="H26" s="8">
-        <v>517</v>
-      </c>
-      <c r="I26" s="6">
+      <c r="F26" s="4">
+        <v>325</v>
+      </c>
+      <c r="G26" s="5">
+        <v>540</v>
+      </c>
+      <c r="H26" s="6">
+        <v>36</v>
+      </c>
+      <c r="I26" s="4">
         <v>179</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="5">
         <v>394</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26" s="6">
         <v>22</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="4">
         <v>249</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="5">
         <v>577</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="6">
         <v>27</v>
       </c>
-      <c r="F27" s="6">
-        <v>548</v>
-      </c>
-      <c r="G27" s="7">
-        <v>876</v>
-      </c>
-      <c r="H27" s="8">
-        <v>529</v>
-      </c>
-      <c r="I27" s="6">
+      <c r="F27" s="4">
+        <v>244</v>
+      </c>
+      <c r="G27" s="5">
+        <v>572</v>
+      </c>
+      <c r="H27" s="6">
+        <v>46</v>
+      </c>
+      <c r="I27" s="4">
         <v>247</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="5">
         <v>575</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27" s="6">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="4">
         <v>171</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="5">
         <v>480</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="6">
         <v>32</v>
       </c>
-      <c r="F28" s="6">
-        <v>556</v>
-      </c>
-      <c r="G28" s="7">
-        <v>865</v>
-      </c>
-      <c r="H28" s="8">
-        <v>542</v>
-      </c>
-      <c r="I28" s="6">
+      <c r="F28" s="4">
+        <v>223</v>
+      </c>
+      <c r="G28" s="5">
+        <v>532</v>
+      </c>
+      <c r="H28" s="6">
+        <v>71</v>
+      </c>
+      <c r="I28" s="4">
         <v>151</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="5">
         <v>460</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28" s="6">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="14">
+        <f>AVERAGE(C21:C28)</f>
         <v>175.5</v>
       </c>
-      <c r="D29" s="11">
-        <v>511.63</v>
-      </c>
-      <c r="E29" s="12">
+      <c r="D29" s="15">
+        <f>AVERAGE(D21:D28)</f>
+        <v>511.625</v>
+      </c>
+      <c r="E29" s="16">
+        <f>AVERAGE(E21:E28)</f>
         <v>15.75</v>
       </c>
-      <c r="F29" s="10">
-        <v>293.25</v>
-      </c>
-      <c r="G29" s="11">
-        <v>629.38</v>
-      </c>
-      <c r="H29" s="12">
-        <v>264</v>
-      </c>
-      <c r="I29" s="10">
+      <c r="F29" s="14">
+        <f>AVERAGE(F21:F28)</f>
+        <v>148</v>
+      </c>
+      <c r="G29" s="15">
+        <f>AVERAGE(G21:G28)</f>
+        <v>484.125</v>
+      </c>
+      <c r="H29" s="16">
+        <f>AVERAGE(H21:H28)</f>
+        <v>24.625</v>
+      </c>
+      <c r="I29" s="14">
+        <f>AVERAGE(I21:I28)</f>
         <v>154</v>
       </c>
-      <c r="J29" s="11">
-        <v>490.13</v>
-      </c>
-      <c r="K29" s="12">
+      <c r="J29" s="15">
+        <f>AVERAGE(J21:J28)</f>
+        <v>490.125</v>
+      </c>
+      <c r="K29" s="16">
+        <f>AVERAGE(K21:K28)</f>
         <v>15.75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F4:H4"/>
     <mergeCell ref="I4:K4"/>
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="I5:K5"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5142,128 +5183,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462F17DC-4DC0-614D-9210-302CFA610163}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.33203125" customWidth="1"/>
     <col min="9" max="15" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>0.85340000000000005</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="8">
         <v>0.82779999999999998</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="8">
         <v>0.77980000000000005</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="8">
         <v>0.9294</v>
       </c>
-      <c r="F2" s="2">
-        <v>0.63129999999999997</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="F2" s="8">
+        <v>0.95840599999999998</v>
+      </c>
+      <c r="G2" s="8">
         <v>0.93730000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>185.25</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>133.5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>150.5</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>175.5</v>
       </c>
-      <c r="F3" s="1">
-        <v>293.25</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="F3" s="4">
+        <v>148</v>
+      </c>
+      <c r="G3" s="4">
         <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>521.37</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <v>469.62</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <v>486.63</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="5">
         <v>511.63</v>
       </c>
-      <c r="F4" s="1">
-        <v>629.38</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="F4" s="5">
+        <v>484.125</v>
+      </c>
+      <c r="G4" s="5">
         <v>490.13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
         <v>24.37</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <v>27.13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="6">
         <v>53.25</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="6">
         <v>15.75</v>
       </c>
-      <c r="F5" s="1">
-        <v>264</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F5" s="6">
+        <v>24.63</v>
+      </c>
+      <c r="G5" s="6">
         <v>15.75</v>
       </c>
     </row>
@@ -5323,7 +5363,7 @@
       <c r="A49" s="1"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="F51" s="3"/>
+      <c r="F51" s="1"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="R54" s="1"/>

</xml_diff>